<commit_message>
conjoint analysis from xlsx
</commit_message>
<xml_diff>
--- a/questionnaire/sources.xlsx
+++ b/questionnaire/sources.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="735" windowWidth="29400" windowHeight="17220"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="29400" windowHeight="17220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Figures" sheetId="1" r:id="rId1"/>
-    <sheet name="Figures (2023)" sheetId="4" r:id="rId2"/>
-    <sheet name="Sources" sheetId="3" r:id="rId3"/>
-    <sheet name="ReadMe" sheetId="2" r:id="rId4"/>
+    <sheet name="Income" sheetId="5" r:id="rId2"/>
+    <sheet name="Policies" sheetId="6" r:id="rId3"/>
+    <sheet name="Figures (2023)" sheetId="4" r:id="rId4"/>
+    <sheet name="Sources" sheetId="3" r:id="rId5"/>
+    <sheet name="ReadMe" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="562">
   <si>
     <t>Country</t>
   </si>
@@ -1356,6 +1358,363 @@
   </si>
   <si>
     <t>GCS_mid: 118 (56% emissions); GCS_low: 117 (25%)</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>d4</t>
+  </si>
+  <si>
+    <t>d5</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>d6</t>
+  </si>
+  <si>
+    <t>d7</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>d8</t>
+  </si>
+  <si>
+    <t>d9</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Staatsschuldenquote auf unter 60% reduzieren</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Rétablissement de l'impôt sur la fortune (ISF)</t>
+  </si>
+  <si>
+    <t>Más necesidades sanitarias dentro del sistema público (cuidado dental, gafas, salud mental)</t>
+  </si>
+  <si>
+    <t>Plan pour l'isolation thermique</t>
+  </si>
+  <si>
+    <t>Inversión en el sistema educativo y universalización de la educación preescolar</t>
+  </si>
+  <si>
+    <t>Plan de redistribution nationale</t>
+  </si>
+  <si>
+    <t>econ_issues</t>
+  </si>
+  <si>
+    <t>Économie</t>
+  </si>
+  <si>
+    <t>Wirtschaftspolitik</t>
+  </si>
+  <si>
+    <t>Asuntos económicos</t>
+  </si>
+  <si>
+    <t>econ1</t>
+  </si>
+  <si>
+    <t>Versement du RSA aux 18-25 ans sans emploi</t>
+  </si>
+  <si>
+    <t>Erhöhung des Regelsatzes des Bürgergelds auf bis zu 600€ pro Monat</t>
+  </si>
+  <si>
+    <t>econ2</t>
+  </si>
+  <si>
+    <t>SMIC à 1600€ net par mois</t>
+  </si>
+  <si>
+    <t>Bürgerversicherung als gerechtere Sozialversicherung</t>
+  </si>
+  <si>
+    <t>Ingreso Básico Garantizado de 600€ al mes</t>
+  </si>
+  <si>
+    <t>econ3</t>
+  </si>
+  <si>
+    <t>Recul de l'âge légal de départ à la retraite à 65 ans</t>
+  </si>
+  <si>
+    <t>Jornada laboral de 34 horas semanales</t>
+  </si>
+  <si>
+    <t>econ4</t>
+  </si>
+  <si>
+    <t>Hausse de 20% du financement de l'hôpital public et de l'Éducation nationale</t>
+  </si>
+  <si>
+    <t>Investitionen für Gigabit-Netzwerke bereitstellen</t>
+  </si>
+  <si>
+    <t>society_issues</t>
+  </si>
+  <si>
+    <t>Démocratie</t>
+  </si>
+  <si>
+    <t>Gesellschaft</t>
+  </si>
+  <si>
+    <t>Asuntos sociales</t>
+  </si>
+  <si>
+    <t>soc1</t>
+  </si>
+  <si>
+    <t>Élection des députés à la proportionnelle</t>
+  </si>
+  <si>
+    <t>Reformar la ley electoral para hacer el Senado más proporcional</t>
+  </si>
+  <si>
+    <t>soc2</t>
+  </si>
+  <si>
+    <t>Référendum d'Initiative Citoyenne (RIC)</t>
+  </si>
+  <si>
+    <t>Cannabis-Legalisierung</t>
+  </si>
+  <si>
+    <t>Abolición de la prostitución</t>
+  </si>
+  <si>
+    <t>climate_pol</t>
+  </si>
+  <si>
+    <t>Climat</t>
+  </si>
+  <si>
+    <t>Klimaschutz</t>
+  </si>
+  <si>
+    <t>Política climática</t>
+  </si>
+  <si>
+    <t>climate1</t>
+  </si>
+  <si>
+    <t>Interdiction des véhicules les plus polluants dans les centres-villes (ZFE)</t>
+  </si>
+  <si>
+    <t>Verpflichtende Solaranlagen auf allen geeigneten Dächern</t>
+  </si>
+  <si>
+    <t>100% de electricidad producida con energías renovables en 2040</t>
+  </si>
+  <si>
+    <t>climate2</t>
+  </si>
+  <si>
+    <t>Plan zur Wärmedämmung</t>
+  </si>
+  <si>
+    <t>Plan de aislamiento térmico</t>
+  </si>
+  <si>
+    <t>climate3</t>
+  </si>
+  <si>
+    <t>Interdiction de la vente de voitures thermiques neuves d'ici 2030</t>
+  </si>
+  <si>
+    <t>Verbot des Verkaufs von Neuwagen mit Verbrennungsmotor bis 2030</t>
+  </si>
+  <si>
+    <t>Prohibir la venta de coches nuevos con motor de combustión para 2030</t>
+  </si>
+  <si>
+    <t>tax_system</t>
+  </si>
+  <si>
+    <t>Fiscalité</t>
+  </si>
+  <si>
+    <t>Steuerpolitik</t>
+  </si>
+  <si>
+    <t>Sistema fiscal</t>
+  </si>
+  <si>
+    <t>tax1</t>
+  </si>
+  <si>
+    <t>Nationales Umverteilungsprogramm</t>
+  </si>
+  <si>
+    <t>Plan de redistribución nacional</t>
+  </si>
+  <si>
+    <t>tax2</t>
+  </si>
+  <si>
+    <t>Die Vermögenssteuer wieder in Kraft setzen</t>
+  </si>
+  <si>
+    <t>Aumentar los impuestos sobre las rentas superiores a 100.000 euros anuales</t>
+  </si>
+  <si>
+    <t>foreign_policy</t>
+  </si>
+  <si>
+    <t>Politique étrangère</t>
+  </si>
+  <si>
+    <t>Außenpolitik</t>
+  </si>
+  <si>
+    <t>Política exterior</t>
+  </si>
+  <si>
+    <t>foreign1</t>
+  </si>
+  <si>
+    <t>Plan mondial pour le climat</t>
+  </si>
+  <si>
+    <t>Globales Klimaprogramm</t>
+  </si>
+  <si>
+    <t>Plan climático global</t>
+  </si>
+  <si>
+    <t>foreign2</t>
+  </si>
+  <si>
+    <t>Taxe mondiale sur les millionaires</t>
+  </si>
+  <si>
+    <t>Globale Steuer auf Millionäre</t>
+  </si>
+  <si>
+    <t>Impuesto mundial a los millonarios</t>
+  </si>
+  <si>
+    <t>foreign3</t>
+  </si>
+  <si>
+    <t>Assemblée démocratique mondiale sur le changement climatique</t>
+  </si>
+  <si>
+    <t>Globale demokratische Versammlung zum Klimawandel</t>
+  </si>
+  <si>
+    <t>Asamblea democrática mundial sobre el cambio climático</t>
+  </si>
+  <si>
+    <t>foreign4</t>
+  </si>
+  <si>
+    <t>Doubler l'aide au développement des pays à faibles revenus</t>
+  </si>
+  <si>
+    <t>Verdoppelung der Mittel für die Entwicklungshilfe in einkommensschwachen Ländern</t>
+  </si>
+  <si>
+    <t>Duplicar la ayuda exterior a los países de renta baja</t>
+  </si>
+  <si>
+    <t>Economic issues</t>
+  </si>
+  <si>
+    <t>Welfare (RSA) payment to unemployed 18-25 year olds</t>
+  </si>
+  <si>
+    <t>Minimum wage (SMIC) at 1600€/month net</t>
+  </si>
+  <si>
+    <t>Raising the legal retirement age to 65</t>
+  </si>
+  <si>
+    <t>20% increase in funding for public hospitals and National Education</t>
+  </si>
+  <si>
+    <t>Institutions</t>
+  </si>
+  <si>
+    <t>Proportional election of MPs</t>
+  </si>
+  <si>
+    <t>Citizens' Initiative Referendum (RIC)</t>
+  </si>
+  <si>
+    <t>Climate policy</t>
+  </si>
+  <si>
+    <t>Prohibition of the most polluting vehicles in city centers (ZFE)</t>
+  </si>
+  <si>
+    <t>Plan for thermal insulation</t>
+  </si>
+  <si>
+    <t>Ban on the sale of new thermal cars by 2030</t>
+  </si>
+  <si>
+    <t>Tax system</t>
+  </si>
+  <si>
+    <t>National redistribution plan</t>
+  </si>
+  <si>
+    <t>Reinstatement of the wealth tax (ISF)</t>
+  </si>
+  <si>
+    <t>Foreign policy</t>
+  </si>
+  <si>
+    <t>Global Climate Plan</t>
+  </si>
+  <si>
+    <t>Global Millionaire Tax</t>
+  </si>
+  <si>
+    <t>Global Democratic Assembly on Climate Change</t>
+  </si>
+  <si>
+    <t>Double foreign aid to low-income countries</t>
+  </si>
+  <si>
+    <t>FR_sources</t>
+  </si>
+  <si>
+    <t>https://www.lemonde.fr/</t>
+  </si>
+  <si>
+    <t>Example (2023)</t>
+  </si>
+  <si>
+    <t>Test (2022)</t>
+  </si>
+  <si>
+    <t>SA_EN</t>
+  </si>
+  <si>
+    <t>IT-CH</t>
+  </si>
+  <si>
+    <t>THIS SHEET IS ONLY MADE OF EXAMPLES</t>
   </si>
 </sst>
 </file>
@@ -1368,7 +1727,7 @@
     <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="167" formatCode="#\ ###\ ###\ ##0;\-#\ ###\ ###\ ##0;0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1457,6 +1816,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1475,11 +1855,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1527,6 +1908,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1534,7 +1919,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1549,12 +1935,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Bluebery PLANTEROSE" id="{B1841E6D-7E30-284D-8D9A-1B2D38EFADD0}" userId="S::bluebery.planterose@sciencespo.fr::b495b69d-f3c3-4357-9166-ef5b6b692f55" providerId="AD"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1818,30 +2198,13 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="Q46" dT="2021-11-30T13:20:27.57" personId="{B1841E6D-7E30-284D-8D9A-1B2D38EFADD0}" id="{45867FEF-B30E-CA46-B729-12C900818755}">
-    <text>2010</text>
-  </threadedComment>
-  <threadedComment ref="S46" dT="2021-11-30T13:20:44.06" personId="{B1841E6D-7E30-284D-8D9A-1B2D38EFADD0}" id="{776472AD-088F-684A-A069-094A5DB506AC}">
-    <text>2019</text>
-  </threadedComment>
-  <threadedComment ref="F47" dT="2021-11-30T13:15:17.52" personId="{B1841E6D-7E30-284D-8D9A-1B2D38EFADD0}" id="{6C4BBD9E-1BCD-3848-B703-E487C8D54720}">
-    <text>2019</text>
-  </threadedComment>
-  <threadedComment ref="I47" dT="2021-11-30T13:16:01.71" personId="{B1841E6D-7E30-284D-8D9A-1B2D38EFADD0}" id="{E01A8FEC-6813-0F4C-A982-DD80F0C4D3CE}">
-    <text>2019</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3831,6 +4194,714 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="4" width="40.5703125" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>454</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>555</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39" t="s">
+        <v>464</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>467</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>536</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>556</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>468</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>470</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>537</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>471</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>473</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>474</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>538</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>558</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>455</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>476</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>477</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>539</v>
+      </c>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40" t="s">
+        <v>478</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="39">
+        <v>21</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="D8" s="23" t="s">
+        <v>561</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>479</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>480</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>540</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39" t="s">
+        <v>481</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>483</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>484</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>541</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>556</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>488</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>486</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>487</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>542</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="39">
+        <v>25</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>558</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="39">
+        <v>26</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
+        <v>490</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>491</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>543</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39" t="s">
+        <v>492</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>494</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>495</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>544</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39" t="s">
+        <v>496</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>459</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>545</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40" t="s">
+        <v>499</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>501</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>502</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>546</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39" t="s">
+        <v>503</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="39">
+        <v>31</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>505</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>506</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>547</v>
+      </c>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39" t="s">
+        <v>507</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
+        <v>509</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>461</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>548</v>
+      </c>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39" t="s">
+        <v>510</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
+        <v>512</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>457</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>549</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="39">
+        <v>35</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="39">
+        <v>36</v>
+      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>515</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>516</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>550</v>
+      </c>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39" t="s">
+        <v>517</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>519</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>520</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>551</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>556</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>521</v>
+      </c>
+      <c r="F26" s="39" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>523</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>524</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>552</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>527</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>553</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>558</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>529</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>531</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>554</v>
+      </c>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40" t="s">
+        <v>533</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="39">
+        <v>42</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="39">
+        <v>43</v>
+      </c>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="39">
+        <v>44</v>
+      </c>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="39">
+        <v>45</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D12" r:id="rId2"/>
+    <hyperlink ref="D27" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R132"/>
   <sheetViews>
@@ -4117,13 +5188,13 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="43" t="s">
         <v>390</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
@@ -6536,7 +7607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I120"/>
   <sheetViews>
@@ -6602,16 +7673,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="43" t="s">
         <v>333</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -7178,14 +8249,14 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
@@ -7239,14 +8310,14 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -8203,7 +9274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>

</xml_diff>

<commit_message>
gcs_high_partial (pb with RU)
</commit_message>
<xml_diff>
--- a/questionnaire/sources.xlsx
+++ b/questionnaire/sources.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="777">
   <si>
     <t>Country</t>
   </si>
@@ -1853,9 +1853,6 @@
     <t>emissions_high_with</t>
   </si>
   <si>
-    <t>map_append</t>
-  </si>
-  <si>
     <t>periodicity_tax</t>
   </si>
   <si>
@@ -2352,6 +2349,18 @@
   </si>
   <si>
     <t>wealth_threshold</t>
+  </si>
+  <si>
+    <t>Net gain per adult\nfollowing the\nGlobal Climate Scheme\nin 2030\n(in % of GDP)</t>
+  </si>
+  <si>
+    <t>gcs_high_legend</t>
+  </si>
+  <si>
+    <t>na_label</t>
+  </si>
+  <si>
+    <t>Non Parties</t>
   </si>
 </sst>
 </file>
@@ -2550,13 +2559,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -5542,10 +5551,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6354,49 +6363,49 @@
       <c r="A17" t="s">
         <v>593</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B17" s="43">
         <v>30</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="43">
         <v>30</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="43">
         <v>30</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="43">
         <v>30</v>
       </c>
-      <c r="F17" s="45">
+      <c r="F17" s="43">
         <v>30</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G17" s="43">
         <v>30</v>
       </c>
-      <c r="H17" s="45">
+      <c r="H17" s="43">
         <v>30</v>
       </c>
-      <c r="I17" s="45">
+      <c r="I17" s="43">
         <v>30</v>
       </c>
-      <c r="J17" s="45">
+      <c r="J17" s="43">
         <v>30</v>
       </c>
-      <c r="K17" s="45">
+      <c r="K17" s="43">
         <v>30</v>
       </c>
-      <c r="L17" s="45">
+      <c r="L17" s="43">
         <v>30</v>
       </c>
-      <c r="M17" s="45">
+      <c r="M17" s="43">
         <v>30</v>
       </c>
-      <c r="N17" s="45">
+      <c r="N17" s="43">
         <v>30</v>
       </c>
-      <c r="O17" s="45">
+      <c r="O17" s="43">
         <v>30</v>
       </c>
-      <c r="P17" s="45">
+      <c r="P17" s="43">
         <v>30</v>
       </c>
     </row>
@@ -6404,49 +6413,49 @@
       <c r="A18" t="s">
         <v>595</v>
       </c>
-      <c r="B18" s="45">
+      <c r="B18" s="43">
         <v>10</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="43">
         <v>10</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="43">
         <v>10</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="43">
         <v>10</v>
       </c>
-      <c r="F18" s="45">
+      <c r="F18" s="43">
         <v>10</v>
       </c>
-      <c r="G18" s="45">
+      <c r="G18" s="43">
         <v>10</v>
       </c>
-      <c r="H18" s="45">
+      <c r="H18" s="43">
         <v>10</v>
       </c>
-      <c r="I18" s="45">
+      <c r="I18" s="43">
         <v>10</v>
       </c>
-      <c r="J18" s="45">
+      <c r="J18" s="43">
         <v>10</v>
       </c>
-      <c r="K18" s="45">
+      <c r="K18" s="43">
         <v>10</v>
       </c>
-      <c r="L18" s="45">
+      <c r="L18" s="43">
         <v>10</v>
       </c>
-      <c r="M18" s="45">
+      <c r="M18" s="43">
         <v>10</v>
       </c>
-      <c r="N18" s="45">
+      <c r="N18" s="43">
         <v>10</v>
       </c>
-      <c r="O18" s="45">
+      <c r="O18" s="43">
         <v>10</v>
       </c>
-      <c r="P18" s="45">
+      <c r="P18" s="43">
         <v>10</v>
       </c>
     </row>
@@ -6454,49 +6463,49 @@
       <c r="A19" t="s">
         <v>596</v>
       </c>
-      <c r="B19" s="45">
+      <c r="B19" s="43">
         <v>40</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="43">
         <v>40</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="43">
         <v>40</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="43">
         <v>40</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="43">
         <v>40</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G19" s="43">
         <v>40</v>
       </c>
-      <c r="H19" s="45">
+      <c r="H19" s="43">
         <v>40</v>
       </c>
-      <c r="I19" s="45">
+      <c r="I19" s="43">
         <v>40</v>
       </c>
-      <c r="J19" s="45">
+      <c r="J19" s="43">
         <v>40</v>
       </c>
-      <c r="K19" s="45">
+      <c r="K19" s="43">
         <v>40</v>
       </c>
-      <c r="L19" s="45">
+      <c r="L19" s="43">
         <v>40</v>
       </c>
-      <c r="M19" s="45">
+      <c r="M19" s="43">
         <v>40</v>
       </c>
-      <c r="N19" s="45">
+      <c r="N19" s="43">
         <v>40</v>
       </c>
-      <c r="O19" s="45">
+      <c r="O19" s="43">
         <v>40</v>
       </c>
-      <c r="P19" s="45">
+      <c r="P19" s="43">
         <v>40</v>
       </c>
     </row>
@@ -6504,455 +6513,455 @@
       <c r="A20" t="s">
         <v>598</v>
       </c>
-      <c r="B20" s="45">
+      <c r="B20" s="43">
         <v>100</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="43">
         <v>100</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="43">
         <v>100</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="43">
         <v>100</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="43">
         <v>100</v>
       </c>
-      <c r="G20" s="45">
+      <c r="G20" s="43">
         <v>100</v>
       </c>
-      <c r="H20" s="45">
+      <c r="H20" s="43">
         <v>100</v>
       </c>
-      <c r="I20" s="45">
+      <c r="I20" s="43">
         <v>100</v>
       </c>
-      <c r="J20" s="45">
+      <c r="J20" s="43">
         <v>100</v>
       </c>
-      <c r="K20" s="45">
+      <c r="K20" s="43">
         <v>100</v>
       </c>
-      <c r="L20" s="45">
+      <c r="L20" s="43">
         <v>100</v>
       </c>
-      <c r="M20" s="45">
+      <c r="M20" s="43">
         <v>100</v>
       </c>
-      <c r="N20" s="45">
+      <c r="N20" s="43">
         <v>100</v>
       </c>
-      <c r="O20" s="45">
+      <c r="O20" s="43">
         <v>100</v>
       </c>
-      <c r="P20" s="45">
+      <c r="P20" s="43">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>607</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>406</v>
-      </c>
-      <c r="C21" s="45" t="s">
-        <v>406</v>
-      </c>
-      <c r="D21" s="45" t="s">
-        <v>406</v>
-      </c>
-      <c r="E21" s="45" t="s">
-        <v>406</v>
-      </c>
-      <c r="F21" s="45" t="s">
-        <v>406</v>
-      </c>
-      <c r="G21" s="45" t="s">
-        <v>408</v>
-      </c>
-      <c r="H21" s="45" t="s">
-        <v>409</v>
-      </c>
-      <c r="I21" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="45" t="s">
-        <v>410</v>
-      </c>
-      <c r="K21" s="45" t="s">
-        <v>411</v>
-      </c>
-      <c r="L21" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="M21" s="45" t="s">
-        <v>409</v>
-      </c>
-      <c r="N21" s="45" t="s">
-        <v>409</v>
-      </c>
-      <c r="O21" s="45" t="s">
-        <v>409</v>
-      </c>
-      <c r="P21" s="45" t="s">
-        <v>7</v>
+        <v>599</v>
+      </c>
+      <c r="B21" t="s">
+        <v>600</v>
+      </c>
+      <c r="C21" t="s">
+        <v>600</v>
+      </c>
+      <c r="D21" t="s">
+        <v>600</v>
+      </c>
+      <c r="E21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F21" t="s">
+        <v>600</v>
+      </c>
+      <c r="G21" t="s">
+        <v>600</v>
+      </c>
+      <c r="H21" t="s">
+        <v>600</v>
+      </c>
+      <c r="I21" t="s">
+        <v>600</v>
+      </c>
+      <c r="J21" t="s">
+        <v>600</v>
+      </c>
+      <c r="K21" t="s">
+        <v>600</v>
+      </c>
+      <c r="L21" t="s">
+        <v>600</v>
+      </c>
+      <c r="M21" t="s">
+        <v>600</v>
+      </c>
+      <c r="N21" t="s">
+        <v>600</v>
+      </c>
+      <c r="O21" t="s">
+        <v>600</v>
+      </c>
+      <c r="P21" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="B22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="D22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="E22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="F22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="G22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H22" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="I22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="J22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="K22" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="L22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="M22" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="N22" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="O22" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="P22" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>602</v>
-      </c>
-      <c r="B23" t="s">
-        <v>603</v>
-      </c>
-      <c r="C23" t="s">
-        <v>603</v>
-      </c>
-      <c r="D23" t="s">
-        <v>603</v>
-      </c>
-      <c r="E23" t="s">
-        <v>603</v>
-      </c>
-      <c r="F23" t="s">
-        <v>603</v>
-      </c>
-      <c r="G23" t="s">
-        <v>603</v>
-      </c>
-      <c r="H23" t="s">
-        <v>604</v>
-      </c>
-      <c r="I23" t="s">
-        <v>603</v>
-      </c>
-      <c r="J23" t="s">
-        <v>603</v>
-      </c>
-      <c r="K23" t="s">
-        <v>604</v>
-      </c>
-      <c r="L23" t="s">
-        <v>603</v>
-      </c>
-      <c r="M23" t="s">
-        <v>604</v>
-      </c>
-      <c r="N23" t="s">
-        <v>604</v>
-      </c>
-      <c r="O23" t="s">
-        <v>604</v>
-      </c>
-      <c r="P23" t="s">
-        <v>603</v>
+        <v>601</v>
+      </c>
+      <c r="B23">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>33</v>
+      </c>
+      <c r="E23">
+        <v>33</v>
+      </c>
+      <c r="F23">
+        <v>33</v>
+      </c>
+      <c r="G23">
+        <v>33</v>
+      </c>
+      <c r="H23">
+        <v>33</v>
+      </c>
+      <c r="I23">
+        <v>33</v>
+      </c>
+      <c r="J23">
+        <v>33</v>
+      </c>
+      <c r="K23">
+        <v>33</v>
+      </c>
+      <c r="L23">
+        <v>33</v>
+      </c>
+      <c r="M23">
+        <v>33</v>
+      </c>
+      <c r="N23">
+        <v>33</v>
+      </c>
+      <c r="O23">
+        <v>33</v>
+      </c>
+      <c r="P23">
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="B24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="F24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="G24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="H24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="I24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="J24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="K24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="L24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="M24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="N24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="O24">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="P24">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="H25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="I25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="J25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="K25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="L25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="M25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="N25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="O25">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="P25">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>606</v>
-      </c>
-      <c r="B26">
-        <v>71</v>
-      </c>
-      <c r="C26">
-        <v>71</v>
-      </c>
-      <c r="D26">
-        <v>71</v>
-      </c>
-      <c r="E26">
-        <v>71</v>
-      </c>
-      <c r="F26">
-        <v>71</v>
-      </c>
-      <c r="G26">
-        <v>71</v>
-      </c>
-      <c r="H26">
-        <v>71</v>
-      </c>
-      <c r="I26">
-        <v>71</v>
-      </c>
-      <c r="J26">
-        <v>71</v>
-      </c>
-      <c r="K26">
-        <v>71</v>
-      </c>
-      <c r="L26">
-        <v>71</v>
-      </c>
-      <c r="M26">
-        <v>71</v>
-      </c>
-      <c r="N26">
-        <v>71</v>
-      </c>
-      <c r="O26">
-        <v>71</v>
-      </c>
-      <c r="P26">
-        <v>71</v>
+        <v>607</v>
+      </c>
+      <c r="B26" t="s">
+        <v>608</v>
+      </c>
+      <c r="C26" t="s">
+        <v>608</v>
+      </c>
+      <c r="D26" t="s">
+        <v>608</v>
+      </c>
+      <c r="E26" t="s">
+        <v>608</v>
+      </c>
+      <c r="F26" t="s">
+        <v>608</v>
+      </c>
+      <c r="G26" t="s">
+        <v>608</v>
+      </c>
+      <c r="H26" t="s">
+        <v>608</v>
+      </c>
+      <c r="I26" t="s">
+        <v>608</v>
+      </c>
+      <c r="J26" t="s">
+        <v>608</v>
+      </c>
+      <c r="K26" t="s">
+        <v>608</v>
+      </c>
+      <c r="L26" t="s">
+        <v>608</v>
+      </c>
+      <c r="M26" t="s">
+        <v>608</v>
+      </c>
+      <c r="N26" t="s">
+        <v>608</v>
+      </c>
+      <c r="O26" t="s">
+        <v>608</v>
+      </c>
+      <c r="P26" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>608</v>
-      </c>
-      <c r="B27" t="s">
-        <v>609</v>
-      </c>
-      <c r="C27" t="s">
-        <v>609</v>
-      </c>
-      <c r="D27" t="s">
-        <v>609</v>
-      </c>
-      <c r="E27" t="s">
-        <v>609</v>
-      </c>
-      <c r="F27" t="s">
-        <v>609</v>
-      </c>
-      <c r="G27" t="s">
-        <v>609</v>
-      </c>
-      <c r="H27" t="s">
-        <v>609</v>
-      </c>
-      <c r="I27" t="s">
-        <v>609</v>
-      </c>
-      <c r="J27" t="s">
-        <v>609</v>
-      </c>
-      <c r="K27" t="s">
-        <v>609</v>
-      </c>
-      <c r="L27" t="s">
-        <v>609</v>
-      </c>
-      <c r="M27" t="s">
-        <v>609</v>
-      </c>
-      <c r="N27" t="s">
-        <v>609</v>
-      </c>
-      <c r="O27" t="s">
-        <v>609</v>
-      </c>
-      <c r="P27" t="s">
-        <v>609</v>
+        <v>615</v>
+      </c>
+      <c r="B27">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>18</v>
+      </c>
+      <c r="F27">
+        <v>18</v>
+      </c>
+      <c r="G27">
+        <v>18</v>
+      </c>
+      <c r="H27">
+        <v>18</v>
+      </c>
+      <c r="I27">
+        <v>18</v>
+      </c>
+      <c r="J27">
+        <v>18</v>
+      </c>
+      <c r="K27">
+        <v>18</v>
+      </c>
+      <c r="L27">
+        <v>18</v>
+      </c>
+      <c r="M27">
+        <v>18</v>
+      </c>
+      <c r="N27">
+        <v>18</v>
+      </c>
+      <c r="O27">
+        <v>18</v>
+      </c>
+      <c r="P27">
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="B28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="J28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="K28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="L28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="N28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="O28">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="P28">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -7005,349 +7014,349 @@
         <v>617</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="P30">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>618</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31">
-        <v>3</v>
-      </c>
-      <c r="F31">
-        <v>3</v>
-      </c>
-      <c r="G31">
-        <v>3</v>
-      </c>
-      <c r="H31">
-        <v>3</v>
-      </c>
-      <c r="I31">
-        <v>3</v>
-      </c>
-      <c r="J31">
-        <v>3</v>
-      </c>
-      <c r="K31">
-        <v>3</v>
-      </c>
-      <c r="L31">
-        <v>3</v>
-      </c>
-      <c r="M31">
-        <v>3</v>
-      </c>
-      <c r="N31">
-        <v>3</v>
-      </c>
-      <c r="O31">
-        <v>3</v>
-      </c>
-      <c r="P31">
-        <v>3</v>
+        <v>612</v>
+      </c>
+      <c r="B31" t="s">
+        <v>625</v>
+      </c>
+      <c r="C31" t="s">
+        <v>636</v>
+      </c>
+      <c r="D31" t="s">
+        <v>637</v>
+      </c>
+      <c r="E31" t="s">
+        <v>638</v>
+      </c>
+      <c r="F31" t="s">
+        <v>639</v>
+      </c>
+      <c r="G31" t="s">
+        <v>640</v>
+      </c>
+      <c r="H31" t="s">
+        <v>641</v>
+      </c>
+      <c r="I31" t="s">
+        <v>642</v>
+      </c>
+      <c r="J31" t="s">
+        <v>643</v>
+      </c>
+      <c r="K31" t="s">
+        <v>644</v>
+      </c>
+      <c r="L31" t="s">
+        <v>645</v>
+      </c>
+      <c r="M31" t="s">
+        <v>646</v>
+      </c>
+      <c r="N31" t="s">
+        <v>647</v>
+      </c>
+      <c r="O31" t="s">
+        <v>648</v>
+      </c>
+      <c r="P31" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>613</v>
+        <v>762</v>
       </c>
       <c r="B32" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C32" t="s">
+        <v>636</v>
+      </c>
+      <c r="D32" t="s">
         <v>637</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>638</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>639</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>640</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>641</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>642</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>643</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>644</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>645</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>646</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>647</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>648</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>649</v>
-      </c>
-      <c r="P32" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>763</v>
+        <v>611</v>
       </c>
       <c r="B33" t="s">
         <v>626</v>
       </c>
       <c r="C33" t="s">
-        <v>637</v>
+        <v>626</v>
       </c>
       <c r="D33" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
       <c r="E33" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="F33" t="s">
-        <v>640</v>
+        <v>626</v>
       </c>
       <c r="G33" t="s">
-        <v>641</v>
+        <v>626</v>
       </c>
       <c r="H33" t="s">
-        <v>642</v>
+        <v>626</v>
       </c>
       <c r="I33" t="s">
-        <v>643</v>
+        <v>626</v>
       </c>
       <c r="J33" t="s">
-        <v>644</v>
+        <v>626</v>
       </c>
       <c r="K33" t="s">
-        <v>645</v>
+        <v>626</v>
       </c>
       <c r="L33" t="s">
-        <v>646</v>
+        <v>626</v>
       </c>
       <c r="M33" t="s">
-        <v>647</v>
+        <v>626</v>
       </c>
       <c r="N33" t="s">
-        <v>648</v>
+        <v>626</v>
       </c>
       <c r="O33" t="s">
-        <v>649</v>
+        <v>626</v>
       </c>
       <c r="P33" t="s">
-        <v>650</v>
+        <v>626</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>612</v>
+        <v>624</v>
       </c>
       <c r="B34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="K34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="L34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="M34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="N34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="O34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="P34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B35" t="s">
         <v>627</v>
       </c>
       <c r="C35" t="s">
-        <v>627</v>
+        <v>650</v>
       </c>
       <c r="D35" t="s">
-        <v>627</v>
+        <v>651</v>
       </c>
       <c r="E35" t="s">
-        <v>627</v>
+        <v>652</v>
       </c>
       <c r="F35" t="s">
-        <v>627</v>
+        <v>653</v>
       </c>
       <c r="G35" t="s">
-        <v>627</v>
+        <v>654</v>
       </c>
       <c r="H35" t="s">
-        <v>627</v>
+        <v>655</v>
       </c>
       <c r="I35" t="s">
-        <v>627</v>
+        <v>656</v>
       </c>
       <c r="J35" t="s">
-        <v>627</v>
+        <v>657</v>
       </c>
       <c r="K35" t="s">
-        <v>627</v>
+        <v>658</v>
       </c>
       <c r="L35" t="s">
-        <v>627</v>
+        <v>659</v>
       </c>
       <c r="M35" t="s">
-        <v>627</v>
+        <v>660</v>
       </c>
       <c r="N35" t="s">
-        <v>627</v>
+        <v>661</v>
       </c>
       <c r="O35" t="s">
-        <v>627</v>
+        <v>662</v>
       </c>
       <c r="P35" t="s">
-        <v>627</v>
+        <v>663</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B36" t="s">
         <v>628</v>
       </c>
       <c r="C36" t="s">
-        <v>651</v>
+        <v>664</v>
       </c>
       <c r="D36" t="s">
-        <v>652</v>
+        <v>665</v>
       </c>
       <c r="E36" t="s">
-        <v>653</v>
+        <v>666</v>
       </c>
       <c r="F36" t="s">
-        <v>654</v>
+        <v>667</v>
       </c>
       <c r="G36" t="s">
-        <v>655</v>
+        <v>668</v>
       </c>
       <c r="H36" t="s">
-        <v>656</v>
+        <v>669</v>
       </c>
       <c r="I36" t="s">
-        <v>657</v>
+        <v>670</v>
       </c>
       <c r="J36" t="s">
-        <v>658</v>
+        <v>671</v>
       </c>
       <c r="K36" t="s">
-        <v>659</v>
+        <v>672</v>
       </c>
       <c r="L36" t="s">
-        <v>660</v>
+        <v>673</v>
       </c>
       <c r="M36" t="s">
-        <v>661</v>
+        <v>674</v>
       </c>
       <c r="N36" t="s">
-        <v>662</v>
+        <v>675</v>
       </c>
       <c r="O36" t="s">
-        <v>663</v>
+        <v>676</v>
       </c>
       <c r="P36" t="s">
-        <v>664</v>
+        <v>677</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -7358,146 +7367,146 @@
         <v>629</v>
       </c>
       <c r="C37" t="s">
-        <v>665</v>
+        <v>678</v>
       </c>
       <c r="D37" t="s">
-        <v>666</v>
+        <v>679</v>
       </c>
       <c r="E37" t="s">
-        <v>667</v>
+        <v>680</v>
       </c>
       <c r="F37" t="s">
-        <v>668</v>
+        <v>681</v>
       </c>
       <c r="G37" t="s">
-        <v>669</v>
+        <v>682</v>
       </c>
       <c r="H37" t="s">
-        <v>670</v>
+        <v>683</v>
       </c>
       <c r="I37" t="s">
-        <v>671</v>
+        <v>684</v>
       </c>
       <c r="J37" t="s">
-        <v>672</v>
+        <v>685</v>
       </c>
       <c r="K37" t="s">
-        <v>673</v>
+        <v>686</v>
       </c>
       <c r="L37" t="s">
-        <v>674</v>
+        <v>687</v>
       </c>
       <c r="M37" t="s">
-        <v>675</v>
+        <v>688</v>
       </c>
       <c r="N37" t="s">
-        <v>676</v>
+        <v>689</v>
       </c>
       <c r="O37" t="s">
-        <v>677</v>
+        <v>690</v>
       </c>
       <c r="P37" t="s">
-        <v>678</v>
+        <v>691</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="B38" t="s">
         <v>630</v>
       </c>
       <c r="C38" t="s">
-        <v>679</v>
+        <v>692</v>
       </c>
       <c r="D38" t="s">
-        <v>680</v>
+        <v>693</v>
       </c>
       <c r="E38" t="s">
-        <v>681</v>
+        <v>694</v>
       </c>
       <c r="F38" t="s">
-        <v>682</v>
+        <v>695</v>
       </c>
       <c r="G38" t="s">
-        <v>683</v>
+        <v>696</v>
       </c>
       <c r="H38" t="s">
-        <v>684</v>
+        <v>697</v>
       </c>
       <c r="I38" t="s">
-        <v>685</v>
+        <v>698</v>
       </c>
       <c r="J38" t="s">
-        <v>686</v>
+        <v>699</v>
       </c>
       <c r="K38" t="s">
-        <v>687</v>
+        <v>700</v>
       </c>
       <c r="L38" t="s">
-        <v>688</v>
+        <v>701</v>
       </c>
       <c r="M38" t="s">
-        <v>689</v>
+        <v>702</v>
       </c>
       <c r="N38" t="s">
-        <v>690</v>
+        <v>703</v>
       </c>
       <c r="O38" t="s">
-        <v>691</v>
+        <v>704</v>
       </c>
       <c r="P38" t="s">
-        <v>692</v>
+        <v>705</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="B39" t="s">
         <v>631</v>
       </c>
       <c r="C39" t="s">
-        <v>693</v>
+        <v>706</v>
       </c>
       <c r="D39" t="s">
-        <v>694</v>
+        <v>707</v>
       </c>
       <c r="E39" t="s">
-        <v>695</v>
+        <v>708</v>
       </c>
       <c r="F39" t="s">
-        <v>696</v>
+        <v>709</v>
       </c>
       <c r="G39" t="s">
-        <v>697</v>
+        <v>710</v>
       </c>
       <c r="H39" t="s">
-        <v>698</v>
+        <v>711</v>
       </c>
       <c r="I39" t="s">
-        <v>699</v>
+        <v>712</v>
       </c>
       <c r="J39" t="s">
-        <v>700</v>
+        <v>713</v>
       </c>
       <c r="K39" t="s">
-        <v>701</v>
+        <v>714</v>
       </c>
       <c r="L39" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="M39" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N39" t="s">
-        <v>704</v>
+        <v>717</v>
       </c>
       <c r="O39" t="s">
-        <v>705</v>
+        <v>718</v>
       </c>
       <c r="P39" t="s">
-        <v>706</v>
+        <v>719</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -7508,296 +7517,296 @@
         <v>632</v>
       </c>
       <c r="C40" t="s">
-        <v>707</v>
+        <v>720</v>
       </c>
       <c r="D40" t="s">
-        <v>708</v>
+        <v>721</v>
       </c>
       <c r="E40" t="s">
-        <v>709</v>
+        <v>722</v>
       </c>
       <c r="F40" t="s">
-        <v>710</v>
+        <v>723</v>
       </c>
       <c r="G40" t="s">
-        <v>711</v>
+        <v>724</v>
       </c>
       <c r="H40" t="s">
-        <v>712</v>
+        <v>725</v>
       </c>
       <c r="I40" t="s">
-        <v>713</v>
+        <v>726</v>
       </c>
       <c r="J40" t="s">
-        <v>714</v>
+        <v>727</v>
       </c>
       <c r="K40" t="s">
-        <v>715</v>
+        <v>728</v>
       </c>
       <c r="L40" t="s">
-        <v>716</v>
+        <v>729</v>
       </c>
       <c r="M40" t="s">
-        <v>717</v>
+        <v>730</v>
       </c>
       <c r="N40" t="s">
-        <v>718</v>
+        <v>731</v>
       </c>
       <c r="O40" t="s">
-        <v>719</v>
+        <v>732</v>
       </c>
       <c r="P40" t="s">
-        <v>720</v>
+        <v>733</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>611</v>
+        <v>623</v>
       </c>
       <c r="B41" t="s">
         <v>633</v>
       </c>
       <c r="C41" t="s">
-        <v>721</v>
+        <v>734</v>
       </c>
       <c r="D41" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
       <c r="E41" t="s">
-        <v>723</v>
+        <v>736</v>
       </c>
       <c r="F41" t="s">
-        <v>724</v>
+        <v>737</v>
       </c>
       <c r="G41" t="s">
-        <v>725</v>
+        <v>738</v>
       </c>
       <c r="H41" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
       <c r="I41" t="s">
-        <v>727</v>
+        <v>740</v>
       </c>
       <c r="J41" t="s">
-        <v>728</v>
+        <v>741</v>
       </c>
       <c r="K41" t="s">
-        <v>729</v>
+        <v>742</v>
       </c>
       <c r="L41" t="s">
-        <v>730</v>
+        <v>743</v>
       </c>
       <c r="M41" t="s">
-        <v>731</v>
+        <v>744</v>
       </c>
       <c r="N41" t="s">
-        <v>732</v>
+        <v>745</v>
       </c>
       <c r="O41" t="s">
-        <v>733</v>
+        <v>746</v>
       </c>
       <c r="P41" t="s">
-        <v>734</v>
+        <v>747</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
       <c r="B42" t="s">
         <v>634</v>
       </c>
       <c r="C42" t="s">
-        <v>735</v>
+        <v>748</v>
       </c>
       <c r="D42" t="s">
-        <v>736</v>
+        <v>749</v>
       </c>
       <c r="E42" t="s">
-        <v>737</v>
+        <v>750</v>
       </c>
       <c r="F42" t="s">
-        <v>738</v>
+        <v>751</v>
       </c>
       <c r="G42" t="s">
-        <v>739</v>
+        <v>752</v>
       </c>
       <c r="H42" t="s">
-        <v>740</v>
+        <v>753</v>
       </c>
       <c r="I42" t="s">
-        <v>741</v>
+        <v>754</v>
       </c>
       <c r="J42" t="s">
-        <v>742</v>
+        <v>755</v>
       </c>
       <c r="K42" t="s">
-        <v>743</v>
+        <v>756</v>
       </c>
       <c r="L42" t="s">
-        <v>744</v>
+        <v>757</v>
       </c>
       <c r="M42" t="s">
-        <v>745</v>
+        <v>758</v>
       </c>
       <c r="N42" t="s">
-        <v>746</v>
+        <v>759</v>
       </c>
       <c r="O42" t="s">
-        <v>747</v>
+        <v>760</v>
       </c>
       <c r="P42" t="s">
-        <v>748</v>
+        <v>761</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
       <c r="B43" t="s">
         <v>635</v>
       </c>
       <c r="C43" t="s">
-        <v>749</v>
+        <v>635</v>
       </c>
       <c r="D43" t="s">
-        <v>750</v>
+        <v>635</v>
       </c>
       <c r="E43" t="s">
-        <v>751</v>
+        <v>635</v>
       </c>
       <c r="F43" t="s">
-        <v>752</v>
+        <v>635</v>
       </c>
       <c r="G43" t="s">
-        <v>753</v>
+        <v>635</v>
       </c>
       <c r="H43" t="s">
-        <v>754</v>
+        <v>635</v>
       </c>
       <c r="I43" t="s">
-        <v>755</v>
+        <v>635</v>
       </c>
       <c r="J43" t="s">
-        <v>756</v>
+        <v>635</v>
       </c>
       <c r="K43" t="s">
-        <v>757</v>
+        <v>635</v>
       </c>
       <c r="L43" t="s">
-        <v>758</v>
+        <v>635</v>
       </c>
       <c r="M43" t="s">
-        <v>759</v>
+        <v>635</v>
       </c>
       <c r="N43" t="s">
-        <v>760</v>
+        <v>635</v>
       </c>
       <c r="O43" t="s">
-        <v>761</v>
+        <v>635</v>
       </c>
       <c r="P43" t="s">
-        <v>762</v>
+        <v>635</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>622</v>
+        <v>763</v>
       </c>
       <c r="B44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="C44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="D44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="E44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="F44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="G44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="H44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="I44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="J44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="K44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="L44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="M44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="N44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="O44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
       <c r="P44" t="s">
-        <v>636</v>
+        <v>764</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="C45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="D45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="E45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="F45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="G45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="H45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="I45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="J45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="K45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="L45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="M45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="N45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="O45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="P45" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -7805,249 +7814,299 @@
         <v>766</v>
       </c>
       <c r="B46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="F46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="G46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="H46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="I46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="J46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="K46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="L46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="M46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="N46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="O46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="P46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>767</v>
-      </c>
-      <c r="B47" t="s">
-        <v>769</v>
-      </c>
-      <c r="C47" t="s">
-        <v>769</v>
-      </c>
-      <c r="D47" t="s">
-        <v>769</v>
-      </c>
-      <c r="E47" t="s">
-        <v>769</v>
-      </c>
-      <c r="F47" t="s">
-        <v>769</v>
-      </c>
-      <c r="G47" t="s">
-        <v>769</v>
-      </c>
-      <c r="H47" t="s">
-        <v>769</v>
-      </c>
-      <c r="I47" t="s">
-        <v>769</v>
-      </c>
-      <c r="J47" t="s">
-        <v>769</v>
-      </c>
-      <c r="K47" t="s">
-        <v>769</v>
-      </c>
-      <c r="L47" t="s">
-        <v>769</v>
-      </c>
-      <c r="M47" t="s">
-        <v>769</v>
-      </c>
-      <c r="N47" t="s">
-        <v>769</v>
-      </c>
-      <c r="O47" t="s">
-        <v>769</v>
-      </c>
-      <c r="P47" t="s">
-        <v>769</v>
+        <v>771</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>2</v>
+      </c>
+      <c r="M47">
+        <v>2</v>
+      </c>
+      <c r="N47">
+        <v>2</v>
+      </c>
+      <c r="O47">
+        <v>2</v>
+      </c>
+      <c r="P47">
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>772</v>
-      </c>
-      <c r="B48">
-        <v>2</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-      <c r="F48">
-        <v>2</v>
-      </c>
-      <c r="G48">
-        <v>2</v>
-      </c>
-      <c r="H48">
-        <v>2</v>
-      </c>
-      <c r="I48">
-        <v>2</v>
-      </c>
-      <c r="J48">
-        <v>2</v>
-      </c>
-      <c r="K48">
-        <v>2</v>
-      </c>
-      <c r="L48">
-        <v>2</v>
-      </c>
-      <c r="M48">
-        <v>2</v>
-      </c>
-      <c r="N48">
-        <v>2</v>
-      </c>
-      <c r="O48">
-        <v>2</v>
-      </c>
-      <c r="P48">
-        <v>2</v>
+        <v>767</v>
+      </c>
+      <c r="B48" t="s">
+        <v>770</v>
+      </c>
+      <c r="C48" t="s">
+        <v>770</v>
+      </c>
+      <c r="D48" t="s">
+        <v>770</v>
+      </c>
+      <c r="E48" t="s">
+        <v>770</v>
+      </c>
+      <c r="F48" t="s">
+        <v>770</v>
+      </c>
+      <c r="G48" t="s">
+        <v>770</v>
+      </c>
+      <c r="H48" t="s">
+        <v>770</v>
+      </c>
+      <c r="I48" t="s">
+        <v>770</v>
+      </c>
+      <c r="J48" t="s">
+        <v>770</v>
+      </c>
+      <c r="K48" t="s">
+        <v>770</v>
+      </c>
+      <c r="L48" t="s">
+        <v>770</v>
+      </c>
+      <c r="M48" t="s">
+        <v>770</v>
+      </c>
+      <c r="N48" t="s">
+        <v>770</v>
+      </c>
+      <c r="O48" t="s">
+        <v>770</v>
+      </c>
+      <c r="P48" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="B49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="C49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="D49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="E49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="F49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="G49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="H49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="I49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="J49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="K49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="L49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="M49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="N49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="O49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
       <c r="P49" t="s">
-        <v>771</v>
+        <v>635</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>774</v>
+      </c>
+      <c r="B50" t="s">
         <v>773</v>
       </c>
-      <c r="B50" t="s">
-        <v>636</v>
-      </c>
       <c r="C50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="D50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="E50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="F50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="G50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="H50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="I50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="J50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="K50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="L50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="M50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="N50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="O50" t="s">
-        <v>636</v>
+        <v>773</v>
       </c>
       <c r="P50" t="s">
-        <v>636</v>
+        <v>773</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>775</v>
+      </c>
+      <c r="B51" t="s">
+        <v>776</v>
+      </c>
+      <c r="C51" t="s">
+        <v>776</v>
+      </c>
+      <c r="D51" t="s">
+        <v>776</v>
+      </c>
+      <c r="E51" t="s">
+        <v>776</v>
+      </c>
+      <c r="F51" t="s">
+        <v>776</v>
+      </c>
+      <c r="G51" t="s">
+        <v>776</v>
+      </c>
+      <c r="H51" t="s">
+        <v>776</v>
+      </c>
+      <c r="I51" t="s">
+        <v>776</v>
+      </c>
+      <c r="J51" t="s">
+        <v>776</v>
+      </c>
+      <c r="K51" t="s">
+        <v>776</v>
+      </c>
+      <c r="L51" t="s">
+        <v>776</v>
+      </c>
+      <c r="M51" t="s">
+        <v>776</v>
+      </c>
+      <c r="N51" t="s">
+        <v>776</v>
+      </c>
+      <c r="O51" t="s">
+        <v>776</v>
+      </c>
+      <c r="P51" t="s">
+        <v>776</v>
       </c>
     </row>
   </sheetData>
@@ -8342,13 +8401,13 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="44" t="s">
         <v>390</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
@@ -10827,16 +10886,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="44" t="s">
         <v>333</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -11403,14 +11462,14 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
@@ -11464,14 +11523,14 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">

</xml_diff>

<commit_message>
maps fixed low and trad PL
</commit_message>
<xml_diff>
--- a/questionnaire/sources.xlsx
+++ b/questionnaire/sources.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2904" uniqueCount="1628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="1639">
   <si>
     <t>Country</t>
   </si>
@@ -4917,6 +4917,39 @@
   </si>
   <si>
     <t>$250</t>
+  </si>
+  <si>
+    <t>name_gcs</t>
+  </si>
+  <si>
+    <t>Globalny Program Klimatyczny</t>
+  </si>
+  <si>
+    <t>Global Climate Scheme</t>
+  </si>
+  <si>
+    <t>participating</t>
+  </si>
+  <si>
+    <t>Pays participant</t>
+  </si>
+  <si>
+    <t>Kraj uczestniczący</t>
+  </si>
+  <si>
+    <t>Participating country</t>
+  </si>
+  <si>
+    <t>potential_party</t>
+  </si>
+  <si>
+    <t>Pays participant potentiel</t>
+  </si>
+  <si>
+    <t>Potencjalny kraj uczestniczący</t>
+  </si>
+  <si>
+    <t>Potential participating country</t>
   </si>
 </sst>
 </file>
@@ -11600,11 +11633,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z89"/>
+  <dimension ref="A1:Z92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A90" sqref="A90:Z92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15997,6 +16030,66 @@
       </c>
       <c r="P89" t="s">
         <v>1523</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B90" t="s">
+        <v>375</v>
+      </c>
+      <c r="E90" t="s">
+        <v>1629</v>
+      </c>
+      <c r="G90" t="s">
+        <v>1630</v>
+      </c>
+      <c r="L90" t="s">
+        <v>1630</v>
+      </c>
+      <c r="M90" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1633</v>
+      </c>
+      <c r="G91" t="s">
+        <v>1634</v>
+      </c>
+      <c r="L91" t="s">
+        <v>1634</v>
+      </c>
+      <c r="M91" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1636</v>
+      </c>
+      <c r="E92" t="s">
+        <v>1637</v>
+      </c>
+      <c r="G92" t="s">
+        <v>1638</v>
+      </c>
+      <c r="L92" t="s">
+        <v>1638</v>
+      </c>
+      <c r="M92" t="s">
+        <v>1636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run prepare & render with final data
</commit_message>
<xml_diff>
--- a/questionnaire/sources.xlsx
+++ b/questionnaire/sources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="732" windowWidth="12960" windowHeight="5868" tabRatio="742"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="12960" windowHeight="5865" tabRatio="742" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Figures" sheetId="1" r:id="rId1"/>
@@ -9467,26 +9467,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B55" sqref="B55"/>
       <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1">
@@ -13163,28 +13163,28 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" style="32" customWidth="1"/>
-    <col min="2" max="2" width="2.88671875" style="32" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="32" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="32" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="32" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="32" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="32" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="32" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="32" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="32" customWidth="1"/>
     <col min="8" max="8" width="20" style="32" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" style="32" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="32" customWidth="1"/>
     <col min="10" max="10" width="13" style="32" customWidth="1"/>
-    <col min="11" max="11" width="20.5546875" style="32" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="32" customWidth="1"/>
-    <col min="13" max="15" width="13.109375" style="32" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" style="32" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" style="32" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="32" customWidth="1"/>
-    <col min="19" max="19" width="13.109375" style="32" customWidth="1"/>
-    <col min="20" max="20" width="9.33203125" style="32" customWidth="1"/>
-    <col min="21" max="22" width="13.109375" style="32" customWidth="1"/>
-    <col min="23" max="16384" width="12.5546875" style="32"/>
+    <col min="11" max="11" width="20.5703125" style="32" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="32" customWidth="1"/>
+    <col min="13" max="15" width="13.140625" style="32" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" style="32" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="32" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="32" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" style="32" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" style="32" customWidth="1"/>
+    <col min="21" max="22" width="13.140625" style="32" customWidth="1"/>
+    <col min="23" max="16384" width="12.5703125" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -27133,19 +27133,19 @@
       <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1">
@@ -28013,7 +28013,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="28.8">
+    <row r="27" spans="1:18" ht="30">
       <c r="A27" s="52" t="s">
         <v>1110</v>
       </c>
@@ -30267,22 +30267,22 @@
       <selection pane="topRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" customWidth="1"/>
-    <col min="8" max="8" width="25.109375" customWidth="1"/>
-    <col min="9" max="10" width="26.44140625" customWidth="1"/>
-    <col min="11" max="11" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="9" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="11" width="39.28515625" customWidth="1"/>
     <col min="12" max="13" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -30978,7 +30978,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="13.95" customHeight="1">
+    <row r="17" spans="1:18" ht="13.9" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>2052</v>
       </c>
@@ -31084,7 +31084,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="14.4" customHeight="1">
+    <row r="19" spans="1:18" ht="14.45" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>2054</v>
       </c>
@@ -31732,10 +31732,10 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -36254,9 +36254,9 @@
       <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -41539,7 +41539,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="403.2">
+    <row r="103" spans="1:17" ht="409.5">
       <c r="A103" s="39" t="s">
         <v>2291</v>
       </c>
@@ -41571,9 +41571,9 @@
       <selection pane="bottomLeft" activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -46858,51 +46858,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI36"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L13" sqref="L13:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="6" width="5.33203125" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" customWidth="1"/>
+    <col min="5" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" customWidth="1"/>
     <col min="8" max="8" width="5" customWidth="1"/>
-    <col min="9" max="9" width="5.109375" customWidth="1"/>
-    <col min="10" max="11" width="5.44140625" customWidth="1"/>
-    <col min="12" max="12" width="4.88671875" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" customWidth="1"/>
-    <col min="14" max="14" width="5.33203125" customWidth="1"/>
-    <col min="15" max="15" width="5.44140625" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" customWidth="1"/>
-    <col min="17" max="17" width="5.5546875" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" customWidth="1"/>
+    <col min="10" max="11" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" customWidth="1"/>
     <col min="18" max="19" width="5" customWidth="1"/>
-    <col min="20" max="20" width="4.5546875" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" customWidth="1"/>
-    <col min="22" max="22" width="4.5546875" customWidth="1"/>
-    <col min="23" max="23" width="5.33203125" customWidth="1"/>
-    <col min="24" max="25" width="4.5546875" customWidth="1"/>
-    <col min="26" max="26" width="4.88671875" customWidth="1"/>
-    <col min="27" max="28" width="5.109375" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" customWidth="1"/>
-    <col min="31" max="31" width="5.5546875" customWidth="1"/>
-    <col min="32" max="32" width="8.5546875" customWidth="1"/>
-    <col min="33" max="33" width="8.44140625" customWidth="1"/>
-    <col min="34" max="35" width="8.33203125" customWidth="1"/>
-    <col min="36" max="36" width="8.44140625" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" customWidth="1"/>
+    <col min="22" max="22" width="4.5703125" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" customWidth="1"/>
+    <col min="24" max="25" width="4.5703125" customWidth="1"/>
+    <col min="26" max="26" width="4.85546875" customWidth="1"/>
+    <col min="27" max="28" width="5.140625" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" customWidth="1"/>
+    <col min="31" max="31" width="5.5703125" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" customWidth="1"/>
+    <col min="33" max="33" width="8.42578125" customWidth="1"/>
+    <col min="34" max="35" width="8.28515625" customWidth="1"/>
+    <col min="36" max="36" width="8.42578125" customWidth="1"/>
     <col min="37" max="37" width="5" customWidth="1"/>
-    <col min="38" max="39" width="6.109375" customWidth="1"/>
-    <col min="40" max="40" width="6.5546875" customWidth="1"/>
-    <col min="41" max="42" width="6.44140625" customWidth="1"/>
-    <col min="43" max="43" width="7.33203125" customWidth="1"/>
-    <col min="44" max="44" width="6.88671875" customWidth="1"/>
-    <col min="45" max="45" width="7.109375" customWidth="1"/>
-    <col min="46" max="47" width="10.44140625" customWidth="1"/>
+    <col min="38" max="39" width="6.140625" customWidth="1"/>
+    <col min="40" max="40" width="6.5703125" customWidth="1"/>
+    <col min="41" max="42" width="6.42578125" customWidth="1"/>
+    <col min="43" max="43" width="7.28515625" customWidth="1"/>
+    <col min="44" max="44" width="6.85546875" customWidth="1"/>
+    <col min="45" max="45" width="7.140625" customWidth="1"/>
+    <col min="46" max="47" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" s="58" customFormat="1" ht="42.75" customHeight="1">
@@ -47369,11 +47369,10 @@
         <v>164</v>
       </c>
       <c r="BD3" s="58">
-        <v>401</v>
+        <v>425</v>
       </c>
       <c r="BE3" s="58">
-        <f>1000-SUM(BA3:BD3)</f>
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:61">
@@ -47418,13 +47417,13 @@
         <v>247</v>
       </c>
       <c r="O4" s="36">
-        <v>373</v>
+        <v>413</v>
       </c>
       <c r="P4" s="36">
         <v>363</v>
       </c>
       <c r="Q4" s="36">
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="R4" s="36">
         <v>250</v>
@@ -47523,11 +47522,10 @@
         <v>150</v>
       </c>
       <c r="BD4">
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="BE4" s="58">
-        <f t="shared" ref="BE4:BE15" si="0">1000-SUM(BA4:BD4)</f>
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="BF4" t="s">
         <v>691</v>
@@ -47682,8 +47680,7 @@
         <v>485</v>
       </c>
       <c r="BE5" s="58">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="BF5" t="s">
         <v>686</v>
@@ -47835,8 +47832,7 @@
         <v>175</v>
       </c>
       <c r="BE6" s="58">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF6" t="s">
         <v>686</v>
@@ -47985,7 +47981,6 @@
         <v>517</v>
       </c>
       <c r="BE7" s="58">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -48279,7 +48274,6 @@
         <v>536</v>
       </c>
       <c r="BE9" s="58">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="BF9" t="s">
@@ -48435,7 +48429,6 @@
         <v>403</v>
       </c>
       <c r="BE10" s="58">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="BF10" t="s">
@@ -48584,8 +48577,7 @@
         <v>533</v>
       </c>
       <c r="BE11" s="58">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:61">
@@ -48623,7 +48615,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="4">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="N12" s="4">
         <v>324</v>
@@ -48672,9 +48664,6 @@
       <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
       <c r="AJ12" s="4"/>
-      <c r="AL12">
-        <v>0</v>
-      </c>
       <c r="AM12">
         <v>44</v>
       </c>
@@ -48721,7 +48710,6 @@
         <v>462</v>
       </c>
       <c r="BE12" s="58">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -48756,14 +48744,14 @@
       <c r="K13" s="48">
         <v>207</v>
       </c>
-      <c r="L13" s="4">
-        <v>69</v>
-      </c>
-      <c r="M13" s="4">
-        <v>439</v>
-      </c>
-      <c r="N13" s="4">
-        <v>196</v>
+      <c r="L13" s="36">
+        <v>98</v>
+      </c>
+      <c r="M13" s="36">
+        <v>624</v>
+      </c>
+      <c r="N13" s="36">
+        <v>278</v>
       </c>
       <c r="O13" s="48">
         <v>749</v>
@@ -49036,7 +49024,7 @@
         <v>137</v>
       </c>
       <c r="AD15" s="6">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="AE15" s="6"/>
       <c r="AF15" s="48"/>
@@ -49094,7 +49082,6 @@
         <v>365</v>
       </c>
       <c r="BE15" s="58">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="BF15" t="s">
@@ -50219,18 +50206,18 @@
       <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
     <col min="11" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -51533,7 +51520,7 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
@@ -53514,7 +53501,7 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
@@ -54755,26 +54742,26 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="4" style="48" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" style="48" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
-    <col min="6" max="6" width="3.33203125" style="48" customWidth="1"/>
-    <col min="7" max="7" width="33.44140625" customWidth="1"/>
-    <col min="8" max="8" width="3.44140625" customWidth="1"/>
-    <col min="9" max="9" width="46.6640625" customWidth="1"/>
-    <col min="10" max="10" width="3.6640625" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" customWidth="1"/>
-    <col min="13" max="13" width="27.44140625" customWidth="1"/>
-    <col min="14" max="14" width="3.44140625" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="48" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" customWidth="1"/>
+    <col min="9" max="9" width="46.7109375" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" customWidth="1"/>
+    <col min="14" max="14" width="3.42578125" customWidth="1"/>
     <col min="15" max="15" width="37" customWidth="1"/>
-    <col min="16" max="16" width="3.6640625" customWidth="1"/>
-    <col min="17" max="17" width="35.6640625" customWidth="1"/>
-    <col min="18" max="18" width="3.44140625" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" customWidth="1"/>
+    <col min="17" max="17" width="35.7109375" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -55948,14 +55935,14 @@
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="27" style="48" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" style="48" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="48"/>
+    <col min="3" max="3" width="27.140625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -57757,7 +57744,7 @@
       <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
latent var, preferred policies by party, features in heatmaps
</commit_message>
<xml_diff>
--- a/questionnaire/sources.xlsx
+++ b/questionnaire/sources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="735" windowWidth="12960" windowHeight="5865" tabRatio="742" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="12960" windowHeight="5865" tabRatio="742" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Figures" sheetId="1" r:id="rId1"/>
@@ -9481,7 +9481,7 @@
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B55" sqref="B55"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -29333,15 +29333,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N23" r:id="rId1"/>
@@ -43916,10 +43916,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K25" sqref="K25"/>
-      <selection pane="bottomLeft" activeCell="H82" sqref="H82"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -45312,7 +45312,7 @@
         <v>1140</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>1141</v>
+        <v>1093</v>
       </c>
       <c r="C27" s="39" t="s">
         <v>1089</v>
@@ -55108,7 +55108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
App C: features, keywords
</commit_message>
<xml_diff>
--- a/questionnaire/sources.xlsx
+++ b/questionnaire/sources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="735" windowWidth="12960" windowHeight="5865" tabRatio="742" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="12960" windowHeight="5865" tabRatio="742"/>
   </bookViews>
   <sheets>
     <sheet name="Figures" sheetId="1" r:id="rId1"/>
@@ -1182,7 +1182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6929" uniqueCount="2485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6931" uniqueCount="2486">
   <si>
     <t>Country</t>
   </si>
@@ -8639,6 +8639,9 @@
   </si>
   <si>
     <t>Centre</t>
+  </si>
+  <si>
+    <t>Expenses NCS</t>
   </si>
 </sst>
 </file>
@@ -9476,12 +9479,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X157"/>
+  <dimension ref="A1:X158"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B55" sqref="B55"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43:M43"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -11744,7 +11747,7 @@
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="2" t="s">
-        <v>1197</v>
+        <v>2485</v>
       </c>
       <c r="B56" s="35"/>
       <c r="C56" s="35">
@@ -11793,164 +11796,187 @@
       </c>
     </row>
     <row r="57" spans="1:18">
-      <c r="A57"/>
-      <c r="B57" s="2"/>
+      <c r="A57" s="2" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B57" s="35"/>
+      <c r="C57" s="35">
+        <v>35</v>
+      </c>
+      <c r="D57" s="35">
+        <v>65</v>
+      </c>
+      <c r="E57" s="35">
+        <v>35</v>
+      </c>
+      <c r="F57" s="35">
+        <v>235</v>
+      </c>
+      <c r="G57" s="35">
+        <v>35</v>
+      </c>
+      <c r="H57" s="35">
+        <v>35</v>
+      </c>
+      <c r="I57" s="35">
+        <v>35</v>
+      </c>
+      <c r="J57" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="K57" s="35">
+        <v>5500</v>
+      </c>
+      <c r="L57" s="35">
+        <v>510</v>
+      </c>
+      <c r="M57" s="35">
+        <v>125</v>
+      </c>
     </row>
     <row r="58" spans="1:18">
-      <c r="A58" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="B58" s="35">
-        <f>(C$3*C58+D$3*D58+E$3*E58+F$3*F58+G$3*G58+H$3*H58+I$3*I58)/5000</f>
-        <v>20.4313</v>
-      </c>
-      <c r="C58" s="35">
-        <v>16.3</v>
-      </c>
-      <c r="D58" s="35">
-        <v>16.7</v>
-      </c>
-      <c r="E58" s="35">
-        <v>34.5</v>
-      </c>
-      <c r="F58" s="35">
-        <v>5.7</v>
-      </c>
-      <c r="G58" s="35">
-        <v>35.799999999999997</v>
-      </c>
-      <c r="H58" s="35">
-        <v>17.8</v>
-      </c>
-      <c r="I58" s="35">
-        <v>13.7</v>
-      </c>
-      <c r="J58" s="35"/>
-      <c r="K58" s="4">
-        <v>10</v>
-      </c>
-      <c r="L58" s="6"/>
-      <c r="M58" s="35">
-        <v>8</v>
-      </c>
-      <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-      <c r="R58" s="2"/>
+      <c r="A58"/>
+      <c r="B58" s="2"/>
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B59" s="35">
         <f>(C$3*C59+D$3*D59+E$3*E59+F$3*F59+G$3*G59+H$3*H59+I$3*I59)/5000</f>
-        <v>40.694020000000009</v>
-      </c>
-      <c r="C59" s="6">
-        <v>41.2</v>
-      </c>
-      <c r="D59" s="6">
-        <v>49.9</v>
-      </c>
-      <c r="E59" s="6">
-        <v>43.9</v>
-      </c>
-      <c r="F59" s="6">
-        <v>56.4</v>
-      </c>
-      <c r="G59" s="6">
-        <v>22.7</v>
-      </c>
-      <c r="H59" s="6">
-        <v>29.5</v>
-      </c>
-      <c r="I59" s="6">
-        <v>40.200000000000003</v>
-      </c>
-      <c r="J59" s="6"/>
+        <v>20.4313</v>
+      </c>
+      <c r="C59" s="35">
+        <v>16.3</v>
+      </c>
+      <c r="D59" s="35">
+        <v>16.7</v>
+      </c>
+      <c r="E59" s="35">
+        <v>34.5</v>
+      </c>
+      <c r="F59" s="35">
+        <v>5.7</v>
+      </c>
+      <c r="G59" s="35">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="H59" s="35">
+        <v>17.8</v>
+      </c>
+      <c r="I59" s="35">
+        <v>13.7</v>
+      </c>
+      <c r="J59" s="35"/>
       <c r="K59" s="4">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="L59" s="6"/>
-      <c r="M59" s="6">
-        <v>41.3</v>
-      </c>
-      <c r="N59" s="10"/>
-      <c r="O59" s="10"/>
-      <c r="P59" s="10"/>
-      <c r="Q59" s="10"/>
+      <c r="M59" s="35">
+        <v>8</v>
+      </c>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2"/>
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B60" s="35">
         <f>(C$3*C60+D$3*D60+E$3*E60+F$3*F60+G$3*G60+H$3*H60+I$3*I60)/5000</f>
-        <v>38.83728</v>
+        <v>40.694020000000009</v>
       </c>
       <c r="C60" s="6">
-        <v>42.4</v>
+        <v>41.2</v>
       </c>
       <c r="D60" s="6">
-        <v>33.4</v>
+        <v>49.9</v>
       </c>
       <c r="E60" s="6">
-        <v>21.6</v>
+        <v>43.9</v>
       </c>
       <c r="F60" s="6">
-        <v>37.9</v>
+        <v>56.4</v>
       </c>
       <c r="G60" s="6">
-        <v>41.4</v>
+        <v>22.7</v>
       </c>
       <c r="H60" s="6">
-        <v>52.7</v>
+        <v>29.5</v>
       </c>
       <c r="I60" s="6">
-        <v>46</v>
-      </c>
-      <c r="J60" s="6">
-        <v>56</v>
-      </c>
+        <v>40.200000000000003</v>
+      </c>
+      <c r="J60" s="6"/>
       <c r="K60" s="4">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="L60" s="6"/>
       <c r="M60" s="6">
-        <v>50.7</v>
-      </c>
+        <v>41.3</v>
+      </c>
+      <c r="N60" s="10"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="B61" s="35">
+        <f>(C$3*C61+D$3*D61+E$3*E61+F$3*F61+G$3*G61+H$3*H61+I$3*I61)/5000</f>
+        <v>38.83728</v>
+      </c>
+      <c r="C61" s="6">
+        <v>42.4</v>
+      </c>
+      <c r="D61" s="6">
+        <v>33.4</v>
+      </c>
+      <c r="E61" s="6">
+        <v>21.6</v>
+      </c>
+      <c r="F61" s="6">
+        <v>37.9</v>
+      </c>
+      <c r="G61" s="6">
+        <v>41.4</v>
+      </c>
+      <c r="H61" s="6">
+        <v>52.7</v>
+      </c>
+      <c r="I61" s="6">
+        <v>46</v>
+      </c>
+      <c r="J61" s="6">
+        <v>56</v>
+      </c>
+      <c r="K61" s="4">
+        <v>28</v>
+      </c>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6">
+        <v>50.7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="A62" s="1" t="s">
         <v>2282</v>
       </c>
-      <c r="B61" s="40"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
-      <c r="H61" s="23"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="23"/>
-      <c r="M61" s="23"/>
-      <c r="N61" s="2"/>
-      <c r="O61" s="2"/>
-      <c r="P61" s="2"/>
-      <c r="Q61" s="2"/>
-      <c r="R61" s="2"/>
-    </row>
-    <row r="62" spans="1:18">
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="32"/>
-      <c r="J62" s="32"/>
-      <c r="M62" s="32"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="30"/>
+      <c r="J62" s="23"/>
+      <c r="M62" s="23"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -11958,773 +11984,771 @@
       <c r="R62" s="2"/>
     </row>
     <row r="63" spans="1:18">
-      <c r="A63" s="1" t="s">
-        <v>1182</v>
-      </c>
-      <c r="B63" s="2"/>
-      <c r="C63" t="s">
-        <v>734</v>
-      </c>
-      <c r="D63" s="32" t="s">
-        <v>710</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>903</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>1144</v>
-      </c>
-      <c r="G63" t="s">
-        <v>740</v>
-      </c>
-      <c r="H63" t="s">
-        <v>716</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>914</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>925</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>2283</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>1496</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>727</v>
-      </c>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="2"/>
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="1" t="s">
-        <v>704</v>
+        <v>1182</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s">
-        <v>735</v>
-      </c>
-      <c r="D64" t="s">
-        <v>711</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>773</v>
+        <v>734</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>710</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>903</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G64" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="H64" t="s">
-        <v>717</v>
-      </c>
-      <c r="I64" t="s">
-        <v>878</v>
+        <v>716</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>914</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>2037</v>
+        <v>925</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>2032</v>
+        <v>1496</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="1" t="s">
-        <v>748</v>
+        <v>704</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s">
-        <v>917</v>
+        <v>735</v>
       </c>
       <c r="D65" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>910</v>
+        <v>773</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G65" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="H65" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I65" t="s">
-        <v>915</v>
+        <v>878</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L65" s="2"/>
+        <v>2284</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>2032</v>
+      </c>
       <c r="M65" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="1" t="s">
-        <v>2042</v>
+        <v>748</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s">
-        <v>736</v>
+        <v>917</v>
       </c>
       <c r="D66" t="s">
-        <v>906</v>
+        <v>712</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>1146</v>
       </c>
       <c r="G66" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H66" t="s">
-        <v>719</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>918</v>
+        <v>718</v>
+      </c>
+      <c r="I66" t="s">
+        <v>915</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L66" s="2" t="s">
-        <v>2034</v>
-      </c>
+        <v>2285</v>
+      </c>
+      <c r="L66" s="2"/>
       <c r="M66" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="1" t="s">
-        <v>1458</v>
-      </c>
-      <c r="B67" s="32"/>
+        <v>2042</v>
+      </c>
+      <c r="B67" s="2"/>
       <c r="C67" t="s">
-        <v>916</v>
+        <v>736</v>
       </c>
       <c r="D67" t="s">
-        <v>713</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>911</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>1147</v>
+        <v>906</v>
       </c>
       <c r="G67" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H67" t="s">
-        <v>720</v>
-      </c>
-      <c r="I67" s="32" t="s">
-        <v>919</v>
-      </c>
-      <c r="J67" s="32" t="s">
-        <v>786</v>
+        <v>719</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>2286</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>2033</v>
-      </c>
-      <c r="M67" s="32" t="s">
-        <v>731</v>
-      </c>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-      <c r="R67" s="2"/>
+        <v>2034</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="68" spans="1:18">
       <c r="A68" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="B68" s="2"/>
+        <v>1458</v>
+      </c>
+      <c r="B68" s="32"/>
+      <c r="C68" t="s">
+        <v>916</v>
+      </c>
       <c r="D68" t="s">
-        <v>905</v>
-      </c>
-      <c r="E68" s="32" t="s">
-        <v>912</v>
+        <v>713</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>911</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>1148</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>2287</v>
+        <v>1147</v>
+      </c>
+      <c r="G68" t="s">
+        <v>744</v>
+      </c>
+      <c r="H68" t="s">
+        <v>720</v>
+      </c>
+      <c r="I68" s="32" t="s">
+        <v>919</v>
+      </c>
+      <c r="J68" s="32" t="s">
+        <v>786</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="M68" s="32" t="s">
-        <v>863</v>
-      </c>
+        <v>731</v>
+      </c>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" t="s">
-        <v>737</v>
+      <c r="D69" t="s">
+        <v>905</v>
       </c>
       <c r="E69" s="32" t="s">
-        <v>913</v>
-      </c>
-      <c r="F69" s="32" t="s">
-        <v>1149</v>
-      </c>
-      <c r="G69" t="s">
-        <v>745</v>
-      </c>
-      <c r="H69" t="s">
-        <v>723</v>
-      </c>
-      <c r="I69" t="s">
-        <v>922</v>
-      </c>
-      <c r="J69" t="s">
-        <v>2040</v>
+        <v>912</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>1148</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>2465</v>
+        <v>2287</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="M69" s="32" t="s">
-        <v>907</v>
+        <v>863</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="A70" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="B70" s="32"/>
+        <v>707</v>
+      </c>
+      <c r="B70" s="2"/>
       <c r="C70" t="s">
-        <v>738</v>
-      </c>
-      <c r="D70" t="s">
-        <v>1949</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>909</v>
+        <v>737</v>
+      </c>
+      <c r="E70" s="32" t="s">
+        <v>913</v>
       </c>
       <c r="F70" s="32" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G70" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="H70" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="I70" t="s">
-        <v>920</v>
-      </c>
-      <c r="J70" s="32" t="s">
-        <v>854</v>
+        <v>922</v>
+      </c>
+      <c r="J70" t="s">
+        <v>2040</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>928</v>
+        <v>2465</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>1497</v>
+        <v>2036</v>
       </c>
       <c r="M70" s="32" t="s">
-        <v>732</v>
-      </c>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
-      <c r="Q70" s="2"/>
-      <c r="R70" s="2"/>
+        <v>907</v>
+      </c>
     </row>
     <row r="71" spans="1:18">
       <c r="A71" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B71" s="32"/>
+      <c r="C71" t="s">
+        <v>738</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1949</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>1150</v>
+      </c>
+      <c r="G71" t="s">
+        <v>746</v>
+      </c>
+      <c r="H71" t="s">
+        <v>722</v>
+      </c>
+      <c r="I71" t="s">
+        <v>920</v>
+      </c>
+      <c r="J71" s="32" t="s">
+        <v>854</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>1497</v>
+      </c>
+      <c r="M71" s="32" t="s">
+        <v>732</v>
+      </c>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+    </row>
+    <row r="72" spans="1:18">
+      <c r="A72" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="B71" s="2"/>
-      <c r="C71" t="s">
+      <c r="B72" s="2"/>
+      <c r="C72" t="s">
         <v>739</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" t="s">
         <v>714</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>904</v>
       </c>
-      <c r="F71" s="32" t="s">
+      <c r="F72" s="32" t="s">
         <v>1151</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G72" t="s">
         <v>747</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H72" t="s">
         <v>721</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I72" t="s">
         <v>921</v>
       </c>
-      <c r="J71" s="32" t="s">
+      <c r="J72" s="32" t="s">
         <v>2041</v>
       </c>
-      <c r="K71" s="32" t="s">
+      <c r="K72" s="32" t="s">
         <v>929</v>
       </c>
-      <c r="L71" s="2" t="s">
+      <c r="L72" s="2" t="s">
         <v>1498</v>
       </c>
-      <c r="M71" s="32" t="s">
+      <c r="M72" s="32" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="72" spans="1:18">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="L72" s="6"/>
-      <c r="M72" s="2"/>
     </row>
     <row r="73" spans="1:18">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="2">
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="1:18">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2">
         <f>52.24+16.68</f>
         <v>68.92</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E74" s="2">
         <v>51.73</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F74" s="2">
         <f>161.44+15.24</f>
         <v>176.68</v>
       </c>
-      <c r="G73" s="2">
+      <c r="G74" s="2">
         <v>58.68</v>
       </c>
-      <c r="H73" s="2">
+      <c r="H74" s="2">
         <v>65.040000000000006</v>
       </c>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2">
+      <c r="I74" s="2"/>
+      <c r="J74" s="2">
         <v>80.16</v>
       </c>
-      <c r="K73" s="2">
+      <c r="K74" s="2">
         <v>112.4</v>
       </c>
-      <c r="L73" s="19">
+      <c r="L74" s="19">
         <v>112.4</v>
       </c>
-      <c r="M73" s="2"/>
-      <c r="O73">
-        <f>SUM(D73:L73)</f>
+      <c r="M74" s="2"/>
+      <c r="O74">
+        <f>SUM(D74:L74)</f>
         <v>726.01</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18">
-      <c r="A74" s="1" t="s">
-        <v>934</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>1772</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>1773</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>1462</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>935</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>1461</v>
-      </c>
-      <c r="K74" t="s">
-        <v>1460</v>
-      </c>
-      <c r="L74" t="s">
-        <v>1459</v>
       </c>
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="1" t="s">
-        <v>1904</v>
+        <v>934</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>1942</v>
+        <v>1772</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>1908</v>
+        <v>1771</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>1905</v>
+        <v>1773</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>1909</v>
+        <v>1462</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>1906</v>
+        <v>935</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>1907</v>
+        <v>1461</v>
+      </c>
+      <c r="K75" t="s">
+        <v>1460</v>
       </c>
       <c r="L75" t="s">
-        <v>1908</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="A76" s="1" t="s">
-        <v>1330</v>
-      </c>
-      <c r="C76" t="s">
-        <v>1332</v>
-      </c>
-      <c r="D76" t="s">
-        <v>1332</v>
-      </c>
-      <c r="E76" t="s">
-        <v>1332</v>
-      </c>
-      <c r="F76" s="48" t="s">
-        <v>1331</v>
-      </c>
-      <c r="G76" t="s">
-        <v>1332</v>
-      </c>
-      <c r="H76" s="48" t="s">
-        <v>1333</v>
-      </c>
-      <c r="I76" s="48" t="s">
-        <v>1339</v>
-      </c>
-      <c r="J76" s="48" t="s">
-        <v>1335</v>
-      </c>
-      <c r="K76" s="48" t="s">
-        <v>1336</v>
+        <v>1904</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>1942</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>1908</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>1905</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>1909</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>1907</v>
       </c>
       <c r="L76" t="s">
-        <v>1332</v>
-      </c>
-      <c r="M76" t="s">
-        <v>1332</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="77" spans="1:18">
       <c r="A77" s="1" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B77" s="2"/>
+        <v>1330</v>
+      </c>
       <c r="C77" t="s">
-        <v>1328</v>
+        <v>1332</v>
       </c>
       <c r="D77" t="s">
-        <v>1328</v>
+        <v>1332</v>
       </c>
       <c r="E77" t="s">
-        <v>1328</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>1329</v>
+        <v>1332</v>
+      </c>
+      <c r="F77" s="48" t="s">
+        <v>1331</v>
       </c>
       <c r="G77" t="s">
-        <v>1328</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>1326</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>1338</v>
-      </c>
-      <c r="J77" t="s">
-        <v>1334</v>
-      </c>
-      <c r="K77" t="s">
-        <v>1337</v>
+        <v>1332</v>
+      </c>
+      <c r="H77" s="48" t="s">
+        <v>1333</v>
+      </c>
+      <c r="I77" s="48" t="s">
+        <v>1339</v>
+      </c>
+      <c r="J77" s="48" t="s">
+        <v>1335</v>
+      </c>
+      <c r="K77" s="48" t="s">
+        <v>1336</v>
       </c>
       <c r="L77" t="s">
-        <v>1327</v>
+        <v>1332</v>
       </c>
       <c r="M77" t="s">
-        <v>1328</v>
-      </c>
-      <c r="N77" t="s">
-        <v>1398</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="78" spans="1:18">
       <c r="A78" s="1" t="s">
-        <v>1407</v>
+        <v>1325</v>
       </c>
       <c r="B78" s="2"/>
-      <c r="C78" s="63" t="s">
-        <v>1408</v>
-      </c>
-      <c r="D78" s="63" t="s">
-        <v>1408</v>
-      </c>
-      <c r="E78" s="63" t="s">
-        <v>1408</v>
-      </c>
-      <c r="F78" s="63" t="s">
-        <v>1408</v>
-      </c>
-      <c r="G78" s="63" t="s">
-        <v>1408</v>
-      </c>
-      <c r="H78" s="63" t="s">
-        <v>1408</v>
-      </c>
-      <c r="I78" s="63" t="s">
-        <v>1408</v>
-      </c>
-      <c r="J78" s="63" t="s">
-        <v>2104</v>
-      </c>
-      <c r="M78" s="63" t="s">
-        <v>1409</v>
+      <c r="C78" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E78" t="s">
+        <v>1328</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G78" t="s">
+        <v>1328</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>1338</v>
+      </c>
+      <c r="J78" t="s">
+        <v>1334</v>
+      </c>
+      <c r="K78" t="s">
+        <v>1337</v>
+      </c>
+      <c r="L78" t="s">
+        <v>1327</v>
+      </c>
+      <c r="M78" t="s">
+        <v>1328</v>
+      </c>
+      <c r="N78" t="s">
+        <v>1398</v>
       </c>
     </row>
     <row r="79" spans="1:18">
       <c r="A79" s="1" t="s">
-        <v>1400</v>
+        <v>1407</v>
       </c>
       <c r="B79" s="2"/>
-      <c r="C79" t="s">
-        <v>1401</v>
-      </c>
-      <c r="D79" t="s">
-        <v>1402</v>
-      </c>
-      <c r="E79" t="s">
-        <v>2092</v>
-      </c>
-      <c r="F79" t="s">
-        <v>1403</v>
-      </c>
-      <c r="G79" t="s">
-        <v>1404</v>
-      </c>
-      <c r="H79" t="s">
-        <v>1405</v>
-      </c>
-      <c r="I79" t="s">
-        <v>2093</v>
-      </c>
-      <c r="J79" t="s">
-        <v>2094</v>
-      </c>
-      <c r="M79" t="s">
-        <v>1406</v>
+      <c r="C79" s="63" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D79" s="63" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E79" s="63" t="s">
+        <v>1408</v>
+      </c>
+      <c r="F79" s="63" t="s">
+        <v>1408</v>
+      </c>
+      <c r="G79" s="63" t="s">
+        <v>1408</v>
+      </c>
+      <c r="H79" s="63" t="s">
+        <v>1408</v>
+      </c>
+      <c r="I79" s="63" t="s">
+        <v>1408</v>
+      </c>
+      <c r="J79" s="63" t="s">
+        <v>2104</v>
+      </c>
+      <c r="M79" s="63" t="s">
+        <v>1409</v>
       </c>
     </row>
     <row r="80" spans="1:18">
       <c r="A80" s="1" t="s">
-        <v>1463</v>
+        <v>1400</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E80" t="s">
+        <v>2092</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1403</v>
+      </c>
+      <c r="G80" t="s">
+        <v>1404</v>
+      </c>
+      <c r="H80" t="s">
+        <v>1405</v>
+      </c>
+      <c r="I80" t="s">
+        <v>2093</v>
+      </c>
+      <c r="J80" t="s">
+        <v>2094</v>
+      </c>
+      <c r="M80" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
+      <c r="A81" s="1" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="C81" t="s">
         <v>2097</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D81" t="s">
         <v>2098</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E81" t="s">
         <v>2099</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>1466</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G81" t="s">
         <v>2100</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H81" s="2" t="s">
         <v>1465</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I81" t="s">
         <v>2101</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J81" t="s">
         <v>2102</v>
       </c>
-      <c r="L80" t="s">
+      <c r="L81" t="s">
         <v>2103</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="M81" s="2" t="s">
         <v>1464</v>
       </c>
     </row>
-    <row r="81" spans="1:18" s="4" customFormat="1">
-      <c r="A81" s="4" t="s">
+    <row r="82" spans="1:18" s="4" customFormat="1">
+      <c r="A82" s="4" t="s">
         <v>1770</v>
       </c>
-      <c r="C81" s="4">
+      <c r="C82" s="4">
         <v>2</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <v>2</v>
       </c>
-      <c r="E81" s="4">
+      <c r="E82" s="4">
         <v>2</v>
       </c>
-      <c r="F81" s="4">
+      <c r="F82" s="4">
         <v>2</v>
       </c>
-      <c r="G81" s="4">
+      <c r="G82" s="4">
         <v>2</v>
       </c>
-      <c r="H81" s="4">
+      <c r="H82" s="4">
         <v>2</v>
       </c>
-      <c r="J81" s="4">
+      <c r="J82" s="4">
         <v>2</v>
       </c>
-      <c r="L81" s="4">
+      <c r="L82" s="4">
         <v>2</v>
       </c>
-      <c r="M81" s="4">
+      <c r="M82" s="4">
         <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18">
-      <c r="A82" s="1" t="s">
-        <v>2060</v>
-      </c>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2">
-        <v>1</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2">
-        <v>1</v>
-      </c>
-      <c r="F82" s="2">
-        <v>1</v>
-      </c>
-      <c r="G82" s="2">
-        <v>1</v>
-      </c>
-      <c r="H82" s="2">
-        <v>1</v>
-      </c>
-      <c r="I82" s="2">
-        <v>1</v>
-      </c>
-      <c r="J82" s="2">
-        <v>1</v>
-      </c>
-      <c r="L82" s="2">
-        <v>1</v>
-      </c>
-      <c r="M82" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:18">
       <c r="A83" s="1" t="s">
-        <v>2061</v>
-      </c>
-      <c r="B83" s="32"/>
-      <c r="C83" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="D83" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="E83" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F83" s="32"/>
-      <c r="G83" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="H83" s="32"/>
-      <c r="I83" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="J83" s="32">
-        <v>0.5</v>
+        <v>2060</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2">
+        <v>1</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2">
+        <v>1</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1</v>
+      </c>
+      <c r="G83" s="2">
+        <v>1</v>
+      </c>
+      <c r="H83" s="2">
+        <v>1</v>
+      </c>
+      <c r="I83" s="2">
+        <v>1</v>
+      </c>
+      <c r="J83" s="2">
+        <v>1</v>
       </c>
       <c r="L83" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M83" s="32"/>
+        <v>1</v>
+      </c>
+      <c r="M83" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="1:18">
       <c r="A84" s="1" t="s">
+        <v>2061</v>
+      </c>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D84" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E84" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="F84" s="32"/>
+      <c r="G84" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="H84" s="32"/>
+      <c r="I84" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="J84" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="L84" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M84" s="32"/>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="A85" s="1" t="s">
         <v>2062</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>2065</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>2064</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E85" t="s">
         <v>2069</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F85" t="s">
         <v>2095</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" t="s">
         <v>2067</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H85" t="s">
         <v>2091</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I85" t="s">
         <v>2068</v>
       </c>
-      <c r="J84" t="s">
+      <c r="J85" t="s">
         <v>2066</v>
       </c>
-      <c r="L84" t="s">
+      <c r="L85" t="s">
         <v>2063</v>
       </c>
-      <c r="M84" t="s">
+      <c r="M85" t="s">
         <v>2096</v>
       </c>
-    </row>
-    <row r="85" spans="1:18">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="5"/>
-      <c r="L85" s="6"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="6"/>
-      <c r="O85" s="2"/>
-      <c r="P85" s="2"/>
-      <c r="Q85" s="2"/>
-      <c r="R85" s="2"/>
     </row>
     <row r="86" spans="1:18">
       <c r="B86" s="2"/>
@@ -12735,29 +12759,30 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="L86" s="2"/>
+      <c r="J86" s="5"/>
+      <c r="L86" s="6"/>
       <c r="M86" s="2"/>
-      <c r="N86" s="1"/>
-      <c r="O86" s="1"/>
-      <c r="Q86" s="1"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="2"/>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
+      <c r="R86" s="2"/>
     </row>
     <row r="87" spans="1:18">
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="18"/>
-      <c r="H87" s="18"/>
-      <c r="I87" s="18"/>
-      <c r="J87" s="18"/>
-      <c r="L87" s="18"/>
-      <c r="M87" s="18"/>
-      <c r="N87" s="10"/>
-      <c r="O87" s="10"/>
-      <c r="P87" s="10"/>
-      <c r="Q87" s="10"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="Q87" s="1"/>
     </row>
     <row r="88" spans="1:18">
       <c r="B88" s="18"/>
@@ -12771,6 +12796,10 @@
       <c r="J88" s="18"/>
       <c r="L88" s="18"/>
       <c r="M88" s="18"/>
+      <c r="N88" s="10"/>
+      <c r="O88" s="10"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="10"/>
     </row>
     <row r="89" spans="1:18">
       <c r="B89" s="18"/>
@@ -12785,34 +12814,33 @@
       <c r="L89" s="18"/>
       <c r="M89" s="18"/>
     </row>
-    <row r="90" spans="1:18" s="1" customFormat="1"/>
-    <row r="91" spans="1:18" s="1" customFormat="1">
-      <c r="B91" s="31"/>
-      <c r="C91" s="31"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="31"/>
-      <c r="F91" s="31"/>
-      <c r="G91" s="31"/>
-      <c r="H91" s="31"/>
-      <c r="I91" s="31"/>
-      <c r="J91" s="31"/>
-      <c r="M91" s="31"/>
-    </row>
-    <row r="92" spans="1:18">
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="24"/>
-      <c r="I92" s="24"/>
-      <c r="J92" s="24"/>
-      <c r="L92" s="25"/>
-      <c r="M92" s="24"/>
+    <row r="90" spans="1:18">
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+    </row>
+    <row r="91" spans="1:18" s="1" customFormat="1"/>
+    <row r="92" spans="1:18" s="1" customFormat="1">
+      <c r="B92" s="31"/>
+      <c r="C92" s="31"/>
+      <c r="D92" s="31"/>
+      <c r="E92" s="31"/>
+      <c r="F92" s="31"/>
+      <c r="G92" s="31"/>
+      <c r="H92" s="31"/>
+      <c r="I92" s="31"/>
+      <c r="J92" s="31"/>
+      <c r="M92" s="31"/>
     </row>
     <row r="93" spans="1:18">
-      <c r="A93" s="22"/>
       <c r="B93" s="24"/>
       <c r="C93" s="24"/>
       <c r="D93" s="24"/>
@@ -12841,21 +12869,21 @@
     </row>
     <row r="95" spans="1:18">
       <c r="A95" s="22"/>
-      <c r="C95" s="18"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24"/>
+      <c r="J95" s="24"/>
+      <c r="L95" s="25"/>
+      <c r="M95" s="24"/>
     </row>
     <row r="96" spans="1:18">
-      <c r="A96" s="3"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-      <c r="J96" s="2"/>
-      <c r="L96" s="2"/>
-      <c r="M96" s="2"/>
+      <c r="A96" s="22"/>
+      <c r="C96" s="18"/>
     </row>
     <row r="97" spans="1:18">
       <c r="A97" s="3"/>
@@ -12887,31 +12915,31 @@
     </row>
     <row r="99" spans="1:18">
       <c r="A99" s="3"/>
-      <c r="B99" s="31"/>
-      <c r="C99" s="31"/>
-      <c r="D99" s="31"/>
-      <c r="E99" s="31"/>
-      <c r="F99" s="31"/>
-      <c r="G99" s="31"/>
-      <c r="H99" s="31"/>
-      <c r="I99" s="31"/>
-      <c r="J99" s="31"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
       <c r="L99" s="2"/>
-      <c r="M99" s="31"/>
+      <c r="M99" s="2"/>
     </row>
     <row r="100" spans="1:18">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
+      <c r="A100" s="3"/>
+      <c r="B100" s="31"/>
+      <c r="C100" s="31"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="31"/>
+      <c r="F100" s="31"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="31"/>
+      <c r="I100" s="31"/>
+      <c r="J100" s="31"/>
       <c r="L100" s="2"/>
-      <c r="M100" s="2"/>
+      <c r="M100" s="31"/>
     </row>
     <row r="101" spans="1:18">
       <c r="A101" s="2"/>
@@ -12940,11 +12968,6 @@
       <c r="J102" s="2"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
-      <c r="N102" s="2"/>
-      <c r="O102" s="2"/>
-      <c r="P102" s="2"/>
-      <c r="Q102" s="2"/>
-      <c r="R102" s="2"/>
     </row>
     <row r="103" spans="1:18">
       <c r="A103" s="2"/>
@@ -12978,6 +13001,11 @@
       <c r="J104" s="2"/>
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
+      <c r="N104" s="2"/>
+      <c r="O104" s="2"/>
+      <c r="P104" s="2"/>
+      <c r="Q104" s="2"/>
+      <c r="R104" s="2"/>
     </row>
     <row r="105" spans="1:18">
       <c r="A105" s="2"/>
@@ -13048,8 +13076,6 @@
       <c r="J109" s="2"/>
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
-      <c r="N109" s="2"/>
-      <c r="O109" s="2"/>
     </row>
     <row r="110" spans="1:18">
       <c r="A110" s="2"/>
@@ -13064,99 +13090,115 @@
       <c r="J110" s="2"/>
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
-      <c r="N110" s="1"/>
+      <c r="N110" s="2"/>
       <c r="O110" s="2"/>
-      <c r="R110" s="8"/>
     </row>
     <row r="111" spans="1:18">
       <c r="A111" s="2"/>
-      <c r="B111" s="19"/>
-      <c r="C111" s="19"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
-      <c r="G111" s="19"/>
-      <c r="H111" s="19"/>
-      <c r="I111" s="19"/>
-      <c r="J111" s="19"/>
-      <c r="L111" s="19"/>
-      <c r="M111" s="19"/>
-      <c r="N111" s="9"/>
-      <c r="O111" s="9"/>
-      <c r="P111" s="9"/>
-      <c r="Q111" s="9"/>
-      <c r="R111" s="9"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="L111" s="2"/>
+      <c r="M111" s="2"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="2"/>
+      <c r="R111" s="8"/>
     </row>
     <row r="112" spans="1:18">
       <c r="A112" s="2"/>
-      <c r="B112" s="6"/>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="6"/>
-      <c r="F112" s="6"/>
-      <c r="G112" s="6"/>
-      <c r="H112" s="6"/>
-      <c r="I112" s="6"/>
-      <c r="J112" s="6"/>
-      <c r="L112" s="6"/>
-      <c r="M112" s="6"/>
-      <c r="N112" s="4"/>
-      <c r="O112" s="4"/>
-      <c r="P112" s="4"/>
-      <c r="Q112" s="4"/>
-      <c r="R112" s="4"/>
+      <c r="B112" s="19"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="19"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="19"/>
+      <c r="I112" s="19"/>
+      <c r="J112" s="19"/>
+      <c r="L112" s="19"/>
+      <c r="M112" s="19"/>
+      <c r="N112" s="9"/>
+      <c r="O112" s="9"/>
+      <c r="P112" s="9"/>
+      <c r="Q112" s="9"/>
+      <c r="R112" s="9"/>
     </row>
     <row r="113" spans="1:18">
       <c r="A113" s="2"/>
-      <c r="B113" s="20"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="20"/>
-      <c r="H113" s="20"/>
-      <c r="I113" s="20"/>
-      <c r="J113" s="20"/>
-      <c r="L113" s="11"/>
-      <c r="M113" s="20"/>
-      <c r="N113" s="13"/>
-      <c r="O113" s="13"/>
-      <c r="P113" s="13"/>
-      <c r="Q113" s="13"/>
-      <c r="R113" s="13"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
+      <c r="N113" s="4"/>
+      <c r="O113" s="4"/>
+      <c r="P113" s="4"/>
+      <c r="Q113" s="4"/>
+      <c r="R113" s="4"/>
     </row>
     <row r="114" spans="1:18">
       <c r="A114" s="2"/>
-      <c r="B114" s="6"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="6"/>
-      <c r="F114" s="6"/>
-      <c r="G114" s="6"/>
-      <c r="H114" s="6"/>
-      <c r="I114" s="6"/>
-      <c r="J114" s="6"/>
-      <c r="L114" s="2"/>
-      <c r="M114" s="6"/>
-      <c r="O114" s="4"/>
+      <c r="B114" s="20"/>
+      <c r="C114" s="14"/>
+      <c r="D114" s="20"/>
+      <c r="E114" s="20"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="20"/>
+      <c r="H114" s="20"/>
+      <c r="I114" s="20"/>
+      <c r="J114" s="20"/>
+      <c r="L114" s="11"/>
+      <c r="M114" s="20"/>
+      <c r="N114" s="13"/>
+      <c r="O114" s="13"/>
+      <c r="P114" s="13"/>
+      <c r="Q114" s="13"/>
+      <c r="R114" s="13"/>
     </row>
     <row r="115" spans="1:18">
-      <c r="A115" s="16"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
-      <c r="M115" s="2"/>
-    </row>
-    <row r="118" spans="1:18">
-      <c r="L118" s="2"/>
-    </row>
-    <row r="157" s="17" customFormat="1"/>
+      <c r="A115" s="2"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="L115" s="2"/>
+      <c r="M115" s="6"/>
+      <c r="O115" s="4"/>
+    </row>
+    <row r="116" spans="1:18">
+      <c r="A116" s="16"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="M116" s="2"/>
+    </row>
+    <row r="119" spans="1:18">
+      <c r="L119" s="2"/>
+    </row>
+    <row r="158" s="17" customFormat="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N32" r:id="rId1"/>
@@ -29333,15 +29375,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N23" r:id="rId1"/>
@@ -43916,10 +43958,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K25" sqref="K25"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -55143,7 +55185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>

</xml_diff>